<commit_message>
Added additional data viz data
</commit_message>
<xml_diff>
--- a/dataForDatawrapper.xlsx
+++ b/dataForDatawrapper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmgoperations-my.sharepoint.com/personal/andrew_hillman_globaldata_com/Documents/Documents/2022/Medical/Topic/002-covid_therapeutics_USA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew.Hillman\OneDrive - GlobalData PLC\Documents\2022\Medical\Topic\002-covid_therapeutics_USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{577CEF1F-D1D6-4119-8ACC-2738603DD8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D394D3F6-3E62-412D-B06D-B163E1C30516}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC3CCDB-4B48-421A-908E-3FFAAED980E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{5A5F571C-9294-43AD-8EFF-1A4457D427F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="8" xr2:uid="{5A5F571C-9294-43AD-8EFF-1A4457D427F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Graph1-Main" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Graph4" sheetId="5" r:id="rId4"/>
     <sheet name="Graph5" sheetId="6" r:id="rId5"/>
     <sheet name="Graph6" sheetId="7" r:id="rId6"/>
+    <sheet name="Graph7" sheetId="12" r:id="rId7"/>
+    <sheet name="CorrelationData" sheetId="9" r:id="rId8"/>
+    <sheet name="CorrelationCoefficients" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="83">
   <si>
     <t>Kentucky</t>
   </si>
@@ -240,16 +243,65 @@
   </si>
   <si>
     <t>Available courses of Paxlovid per 100,000</t>
+  </si>
+  <si>
+    <t>xVariable</t>
+  </si>
+  <si>
+    <t>yVariable</t>
+  </si>
+  <si>
+    <t>availableCoursesPer100,000</t>
+  </si>
+  <si>
+    <t>casesLastSevenDaysPer100,000</t>
+  </si>
+  <si>
+    <t>TotalAllocations10/02/22</t>
+  </si>
+  <si>
+    <t>TotalPopulation</t>
+  </si>
+  <si>
+    <t>Allocations10/02/22Per100,000</t>
+  </si>
+  <si>
+    <t>Allocated doses (Jan 24 -30)</t>
+  </si>
+  <si>
+    <t>Allocated doses per 100,000 (Jan 24-30)</t>
+  </si>
+  <si>
+    <t>New cases per 100,000 (Jan 18-24)</t>
+  </si>
+  <si>
+    <t>Available courses per 100,000 on Jan 24th</t>
+  </si>
+  <si>
+    <t>Population size</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Available Paxlovid</t>
+  </si>
+  <si>
+    <t>Available Molnupiravir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,16 +309,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -274,21 +345,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FF33CCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2832,8 +3030,8 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3561,4 +3759,1371 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0F1C6F-8999-4106-A90B-83915C46A4C3}">
+  <sheetPr>
+    <tabColor rgb="FFCCFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1"/>
+    <col min="3" max="3" width="32.36328125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>44564</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.777434581424286</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.0180469242325185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>44565</v>
+      </c>
+      <c r="B3" s="3">
+        <v>9.3024533454294112</v>
+      </c>
+      <c r="C3" s="3">
+        <v>21.170006642596007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>44566</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5.1359963948020511</v>
+      </c>
+      <c r="C4" s="3">
+        <v>15.191383455846038</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>44568</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5.2592481051376652</v>
+      </c>
+      <c r="C5" s="3">
+        <v>19.028965793251157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>44571</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6.5683399097171433</v>
+      </c>
+      <c r="C6" s="3">
+        <v>28.007425781313191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>44572</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6.1750937349087183</v>
+      </c>
+      <c r="C7" s="3">
+        <v>34.888166065742375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>44573</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6.4298342748350477</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44.800776393031256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>44574</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7.1550058477750209</v>
+      </c>
+      <c r="C9" s="3">
+        <v>49.121908138559995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>44575</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.5382317256504319</v>
+      </c>
+      <c r="C10" s="3">
+        <v>54.481221988722602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>44580</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12.846855253051041</v>
+      </c>
+      <c r="C11" s="3">
+        <v>73.25880310544764</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>44582</v>
+      </c>
+      <c r="B12" s="3">
+        <v>16.298513299430038</v>
+      </c>
+      <c r="C12" s="3">
+        <v>92.288379055680622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>44585</v>
+      </c>
+      <c r="B13" s="3">
+        <v>17.911158202484614</v>
+      </c>
+      <c r="C13" s="3">
+        <v>103.79532957656828</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>44586</v>
+      </c>
+      <c r="B14" s="3">
+        <v>18.404775200808917</v>
+      </c>
+      <c r="C14" s="3">
+        <v>110.14096218790681</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>44587</v>
+      </c>
+      <c r="B15" s="3">
+        <v>18.124713146135424</v>
+      </c>
+      <c r="C15" s="3">
+        <v>108.94291895402561</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>44588</v>
+      </c>
+      <c r="B16" s="3">
+        <v>17.873938626591176</v>
+      </c>
+      <c r="C16" s="3">
+        <v>113.05385161930383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>44589</v>
+      </c>
+      <c r="B17" s="3">
+        <v>18.937747324463157</v>
+      </c>
+      <c r="C17" s="3">
+        <v>116.02440088548668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>44593</v>
+      </c>
+      <c r="B18" s="3">
+        <v>21.334138870716224</v>
+      </c>
+      <c r="C18" s="3">
+        <v>121.69336940394295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>44596</v>
+      </c>
+      <c r="B19" s="3">
+        <v>26.941481534004687</v>
+      </c>
+      <c r="C19" s="3">
+        <v>137.53853606585142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>44599</v>
+      </c>
+      <c r="B20" s="3">
+        <v>29.592918698675007</v>
+      </c>
+      <c r="C20" s="3">
+        <v>149.14189138987282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>44601</v>
+      </c>
+      <c r="B21" s="3">
+        <v>29.976097283282755</v>
+      </c>
+      <c r="C21" s="3">
+        <v>152.09810196698203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDDF571-EC81-4645-870E-543957CFEC07}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>160.00000000000003</v>
+      </c>
+      <c r="C2" s="1">
+        <v>27.475924221401002</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1958.5182234067397</v>
+      </c>
+      <c r="E2" s="1">
+        <v>17.5159016911431</v>
+      </c>
+      <c r="F2">
+        <v>582328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>479.99999999999977</v>
+      </c>
+      <c r="C3" s="1">
+        <v>26.893965498404</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1763.6278166526315</v>
+      </c>
+      <c r="E3" s="1">
+        <v>27.118081877557401</v>
+      </c>
+      <c r="F3">
+        <v>1784787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>200.00000000000028</v>
+      </c>
+      <c r="C4" s="1">
+        <v>26.133235072369501</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2053.5496119867921</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.3066617536184699</v>
+      </c>
+      <c r="F4">
+        <v>765309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>180.00000000000014</v>
+      </c>
+      <c r="C5" s="1">
+        <v>28.876372229272</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2369.9480385724164</v>
+      </c>
+      <c r="E5" s="1">
+        <v>22.7802492030923</v>
+      </c>
+      <c r="F5">
+        <v>623347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>359.9999999999996</v>
+      </c>
+      <c r="C6" s="1">
+        <v>25.586244834776799</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2128.6334244487939</v>
+      </c>
+      <c r="E6" s="1">
+        <v>20.468995867821501</v>
+      </c>
+      <c r="F6">
+        <v>1407006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>4940.0000000000091</v>
+      </c>
+      <c r="C7" s="1">
+        <v>25.5471749789107</v>
+      </c>
+      <c r="D7" s="1">
+        <v>458.96482433266021</v>
+      </c>
+      <c r="E7" s="1">
+        <v>22.185704586948699</v>
+      </c>
+      <c r="F7">
+        <v>19336776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>919.99999999999864</v>
+      </c>
+      <c r="C8" s="1">
+        <v>25.864448921368101</v>
+      </c>
+      <c r="D8" s="1">
+        <v>852.26170549051653</v>
+      </c>
+      <c r="E8" s="1">
+        <v>13.775630403772199</v>
+      </c>
+      <c r="F8">
+        <v>3557006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>1740.0000000000027</v>
+      </c>
+      <c r="C9" s="1">
+        <v>25.240898262642901</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1983.5284280693877</v>
+      </c>
+      <c r="E9" s="1">
+        <v>26.140286591541599</v>
+      </c>
+      <c r="F9">
+        <v>6893574</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3240.0000000000041</v>
+      </c>
+      <c r="C10" s="1">
+        <v>25.345659250766701</v>
+      </c>
+      <c r="D10" s="1">
+        <v>839.8878720551121</v>
+      </c>
+      <c r="E10" s="1">
+        <v>29.264849153431499</v>
+      </c>
+      <c r="F10">
+        <v>12783254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>359.99999999999972</v>
+      </c>
+      <c r="C11" s="1">
+        <v>26.663881772348201</v>
+      </c>
+      <c r="D11" s="1">
+        <v>524.38967485618173</v>
+      </c>
+      <c r="E11" s="1">
+        <v>25.775085713269899</v>
+      </c>
+      <c r="F11">
+        <v>1350141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>3160.0000000000018</v>
+      </c>
+      <c r="C12" s="1">
+        <v>25.104210277949701</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1393.1327273897261</v>
+      </c>
+      <c r="E12" s="1">
+        <v>19.956258296901801</v>
+      </c>
+      <c r="F12">
+        <v>12587530</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>360</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26.349014656639401</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2140.271907192915</v>
+      </c>
+      <c r="E13" s="1">
+        <v>28.837532707544199</v>
+      </c>
+      <c r="F13">
+        <v>1366275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>2220.0000000000027</v>
+      </c>
+      <c r="C14" s="1">
+        <v>24.993326669196801</v>
+      </c>
+      <c r="D14" s="1">
+        <v>776.32424945996968</v>
+      </c>
+      <c r="E14" s="1">
+        <v>9.9973306676787104</v>
+      </c>
+      <c r="F14">
+        <v>8882371</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>520.0000000000008</v>
+      </c>
+      <c r="C15" s="1">
+        <v>24.687618542110702</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2548.3794240093739</v>
+      </c>
+      <c r="E15" s="1">
+        <v>29.055427976484101</v>
+      </c>
+      <c r="F15">
+        <v>2106319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>2480.0000000000041</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.883221935764201</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1849.2949670171888</v>
+      </c>
+      <c r="E16" s="1">
+        <v>24.873188378531999</v>
+      </c>
+      <c r="F16">
+        <v>9966555</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>179.99999999999966</v>
+      </c>
+      <c r="C17" s="1">
+        <v>24.618481914989601</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2987.9998577598826</v>
+      </c>
+      <c r="E17" s="1">
+        <v>28.3112542022381</v>
+      </c>
+      <c r="F17">
+        <v>731158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>280.00000000000011</v>
+      </c>
+      <c r="C18" s="1">
+        <v>26.4869339009105</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1719.3803949391038</v>
+      </c>
+      <c r="E18" s="1">
+        <v>15.040794608017</v>
+      </c>
+      <c r="F18">
+        <v>1057125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1100.0000000000023</v>
+      </c>
+      <c r="C19" s="1">
+        <v>24.568647145313101</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1751.1191577153036</v>
+      </c>
+      <c r="E19" s="1">
+        <v>17.041707065339899</v>
+      </c>
+      <c r="F19">
+        <v>4477251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>2879.9999999999964</v>
+      </c>
+      <c r="C20" s="1">
+        <v>24.629663504919101</v>
+      </c>
+      <c r="D20" s="1">
+        <v>960.4200452279299</v>
+      </c>
+      <c r="E20" s="1">
+        <v>19.447171809092399</v>
+      </c>
+      <c r="F20">
+        <v>11693217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>1499.9999999999982</v>
+      </c>
+      <c r="C21" s="1">
+        <v>24.769634145898401</v>
+      </c>
+      <c r="D21" s="1">
+        <v>530.15273616937941</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16.744272682627301</v>
+      </c>
+      <c r="F21">
+        <v>6055802</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>1500</v>
+      </c>
+      <c r="C22" s="1">
+        <v>24.384106244477</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1530.2489714783985</v>
+      </c>
+      <c r="E22" s="1">
+        <v>24.595435165262501</v>
+      </c>
+      <c r="F22">
+        <v>6151548</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>1199.9999999999993</v>
+      </c>
+      <c r="C23" s="1">
+        <v>24.382651580849199</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1825.6713559924024</v>
+      </c>
+      <c r="E23" s="1">
+        <v>18.002524417193701</v>
+      </c>
+      <c r="F23">
+        <v>4921532</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1440.0000000000016</v>
+      </c>
+      <c r="C24" s="1">
+        <v>24.688585215480799</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1536.4015186908878</v>
+      </c>
+      <c r="E24" s="1">
+        <v>23.677039015679799</v>
+      </c>
+      <c r="F24">
+        <v>5832655</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25">
+        <v>240.00000000000034</v>
+      </c>
+      <c r="C25" s="1">
+        <v>24.320815882303499</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1176.3167948407443</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>986809</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>9559.9999999999873</v>
+      </c>
+      <c r="C26" s="1">
+        <v>24.283634065142799</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1923.8886897145449</v>
+      </c>
+      <c r="E26" s="1">
+        <v>18.121280901749898</v>
+      </c>
+      <c r="F26">
+        <v>39368078</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>739.99999999999909</v>
+      </c>
+      <c r="C27" s="1">
+        <v>24.9428169069154</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2004.3575775266568</v>
+      </c>
+      <c r="E27" s="1">
+        <v>27.167446522937599</v>
+      </c>
+      <c r="F27">
+        <v>2966786</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>2099.9999999999964</v>
+      </c>
+      <c r="C28" s="1">
+        <v>24.445429246022599</v>
+      </c>
+      <c r="D28" s="1">
+        <v>984.76665615513207</v>
+      </c>
+      <c r="E28" s="1">
+        <v>18.660010991130601</v>
+      </c>
+      <c r="F28">
+        <v>8590563</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1140.0000000000002</v>
+      </c>
+      <c r="C29" s="1">
+        <v>24.540838754203701</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1717.0406848357852</v>
+      </c>
+      <c r="E29" s="1">
+        <v>24.562365805742498</v>
+      </c>
+      <c r="F29">
+        <v>4645318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>1660.0000000000023</v>
+      </c>
+      <c r="C30" s="1">
+        <v>24.103964172796999</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1672.6844294490038</v>
+      </c>
+      <c r="E30" s="1">
+        <v>19.370294100307898</v>
+      </c>
+      <c r="F30">
+        <v>6886834</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>259.99999999999983</v>
+      </c>
+      <c r="C31" s="1">
+        <v>24.061219144956802</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1389.6279487718136</v>
+      </c>
+      <c r="E31" s="1">
+        <v>13.788929433071401</v>
+      </c>
+      <c r="F31">
+        <v>1080577</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>1039.9999999999984</v>
+      </c>
+      <c r="C32" s="1">
+        <v>24.519587024140201</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1812.5397411816132</v>
+      </c>
+      <c r="E32" s="1">
+        <v>9.3598808159458393</v>
+      </c>
+      <c r="F32">
+        <v>4241507</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>1359.999999999998</v>
+      </c>
+      <c r="C33" s="1">
+        <v>24.039557799404701</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1612.029111904495</v>
+      </c>
+      <c r="E33" s="1">
+        <v>19.496788421134902</v>
+      </c>
+      <c r="F33">
+        <v>5657342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>700.00000000000102</v>
+      </c>
+      <c r="C34" s="1">
+        <v>24.0235705546528</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2553.4309948675359</v>
+      </c>
+      <c r="E34" s="1">
+        <v>9.47215067583452</v>
+      </c>
+      <c r="F34">
+        <v>2913805</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>780.00000000000011</v>
+      </c>
+      <c r="C35" s="1">
+        <v>24.655759759334501</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1162.2345831169368</v>
+      </c>
+      <c r="E35" s="1">
+        <v>27.247775528905599</v>
+      </c>
+      <c r="F35">
+        <v>3163561</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>5239.9999999999991</v>
+      </c>
+      <c r="C36" s="1">
+        <v>24.110453114555199</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1057.6666823722035</v>
+      </c>
+      <c r="E36" s="1">
+        <v>7.5552221400953501</v>
+      </c>
+      <c r="F36">
+        <v>21733312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37">
+        <v>2519.9999999999959</v>
+      </c>
+      <c r="C37" s="1">
+        <v>23.771739231944501</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1589.4803639302347</v>
+      </c>
+      <c r="E37" s="1">
+        <v>15.423330811202099</v>
+      </c>
+      <c r="F37">
+        <v>10600823</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38">
+        <v>739.99999999999989</v>
+      </c>
+      <c r="C38" s="1">
+        <v>24.418235538299999</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1884.3288383981373</v>
+      </c>
+      <c r="E38" s="1">
+        <v>20.887490669924201</v>
+      </c>
+      <c r="F38">
+        <v>3030522</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39">
+        <v>460.0000000000004</v>
+      </c>
+      <c r="C39" s="1">
+        <v>23.741298298058599</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1477.1216462835578</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10.3739151258908</v>
+      </c>
+      <c r="F39">
+        <v>1937552</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40">
+        <v>1619.999999999998</v>
+      </c>
+      <c r="C40" s="1">
+        <v>23.982402246174001</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1445.7687566441987</v>
+      </c>
+      <c r="E40" s="1">
+        <v>22.946125605907302</v>
+      </c>
+      <c r="F40">
+        <v>6754953</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41">
+        <v>1819.9999999999984</v>
+      </c>
+      <c r="C41" s="1">
+        <v>23.655988890523702</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2103.7582867448996</v>
+      </c>
+      <c r="E41" s="1">
+        <v>13.582696917910599</v>
+      </c>
+      <c r="F41">
+        <v>7693612</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42">
+        <v>960.00000000000057</v>
+      </c>
+      <c r="C42" s="1">
+        <v>24.1158586137451</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2006.5901607799269</v>
+      </c>
+      <c r="E42" s="1">
+        <v>19.744859240003802</v>
+      </c>
+      <c r="F42">
+        <v>3980783</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43">
+        <v>1360.0000000000023</v>
+      </c>
+      <c r="C43" s="1">
+        <v>23.417110917384299</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1281.0020595004682</v>
+      </c>
+      <c r="E43" s="1">
+        <v>20.6449382278998</v>
+      </c>
+      <c r="F43">
+        <v>5807719</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>1239.9999999999989</v>
+      </c>
+      <c r="C44" s="1">
+        <v>23.763712045135701</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1995.2510904477544</v>
+      </c>
+      <c r="E44" s="1">
+        <v>20.889069459030601</v>
+      </c>
+      <c r="F44">
+        <v>5218040</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45">
+        <v>2500.0000000000041</v>
+      </c>
+      <c r="C45" s="1">
+        <v>23.342633349694999</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1157.729254771491</v>
+      </c>
+      <c r="E45" s="1">
+        <v>15.406138010798699</v>
+      </c>
+      <c r="F45">
+        <v>10710017</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>720.00000000000034</v>
+      </c>
+      <c r="C46" s="1">
+        <v>22.9426570592166</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1834.5840798990778</v>
+      </c>
+      <c r="E46" s="1">
+        <v>12.650326184040299</v>
+      </c>
+      <c r="F46">
+        <v>3138259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47">
+        <v>1699.999999999998</v>
+      </c>
+      <c r="C47" s="1">
+        <v>22.906726101985299</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1959.7916889277374</v>
+      </c>
+      <c r="E47" s="1">
+        <v>20.589104402255</v>
+      </c>
+      <c r="F47">
+        <v>7421401</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48">
+        <v>219.99999999999986</v>
+      </c>
+      <c r="C48" s="1">
+        <v>24.643868101537201</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1725.7428726012836</v>
+      </c>
+      <c r="E48" s="1">
+        <v>13.106057126726601</v>
+      </c>
+      <c r="F48">
+        <v>892717</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>6559.9999999999918</v>
+      </c>
+      <c r="C49" s="1">
+        <v>22.3427466571964</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1303.508536683265</v>
+      </c>
+      <c r="E49" s="1">
+        <v>11.147531983079899</v>
+      </c>
+      <c r="F49">
+        <v>29360759</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50">
+        <v>400.00000000000017</v>
+      </c>
+      <c r="C50" s="1">
+        <v>21.894857609530401</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1105.7997835693325</v>
+      </c>
+      <c r="E50" s="1">
+        <v>9.7432116362410195</v>
+      </c>
+      <c r="F50">
+        <v>1826913</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51">
+        <v>679.99999999999898</v>
+      </c>
+      <c r="C51" s="1">
+        <v>20.9238559343286</v>
+      </c>
+      <c r="D51" s="1">
+        <v>3003.9579935129896</v>
+      </c>
+      <c r="E51" s="1">
+        <v>6.2156160275505599</v>
+      </c>
+      <c r="F51">
+        <v>3249879</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE68B34-216F-45D0-AB9C-A3900E967393}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="10">
+        <f>CORREL(CorrelationData!$B$2:$B$51,CorrelationData!$F$2:$F$51)</f>
+        <v>0.99853900841111332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="10">
+        <f>CORREL(CorrelationData!$C$2:$C$51,CorrelationData!$D$2:$D$51)</f>
+        <v>-5.3457852500284564E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="11">
+        <f>CORREL(CorrelationData!$C$2:$C$51,CorrelationData!$E$2:$E$51)</f>
+        <v>0.35728886057403908</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated R analysis + graph data
</commit_message>
<xml_diff>
--- a/dataForDatawrapper.xlsx
+++ b/dataForDatawrapper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew.Hillman\OneDrive - GlobalData PLC\Documents\2022\Medical\Topic\002-covid_therapeutics_USA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmgoperations-my.sharepoint.com/personal/andrew_hillman_globaldata_com/Documents/Documents/2022/Medical/Topic/002-covid_therapeutics_USA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC3CCDB-4B48-421A-908E-3FFAAED980E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="8_{577CEF1F-D1D6-4119-8ACC-2738603DD8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3338B4D9-5702-423B-BF33-CB26012CEEF9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="8" xr2:uid="{5A5F571C-9294-43AD-8EFF-1A4457D427F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{5A5F571C-9294-43AD-8EFF-1A4457D427F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Graph1-Main" sheetId="4" r:id="rId1"/>
@@ -19,9 +19,8 @@
     <sheet name="Graph4" sheetId="5" r:id="rId4"/>
     <sheet name="Graph5" sheetId="6" r:id="rId5"/>
     <sheet name="Graph6" sheetId="7" r:id="rId6"/>
-    <sheet name="Graph7" sheetId="12" r:id="rId7"/>
-    <sheet name="CorrelationData" sheetId="9" r:id="rId8"/>
-    <sheet name="CorrelationCoefficients" sheetId="11" r:id="rId9"/>
+    <sheet name="CorrelationData" sheetId="9" r:id="rId7"/>
+    <sheet name="CorrelationFigures" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="76">
   <si>
     <t>Kentucky</t>
   </si>
@@ -257,40 +256,19 @@
     <t>casesLastSevenDaysPer100,000</t>
   </si>
   <si>
+    <t>10/02/2022Per100,000</t>
+  </si>
+  <si>
     <t>TotalAllocations10/02/22</t>
   </si>
   <si>
     <t>TotalPopulation</t>
   </si>
   <si>
+    <t>R2</t>
+  </si>
+  <si>
     <t>Allocations10/02/22Per100,000</t>
-  </si>
-  <si>
-    <t>Allocated doses (Jan 24 -30)</t>
-  </si>
-  <si>
-    <t>Allocated doses per 100,000 (Jan 24-30)</t>
-  </si>
-  <si>
-    <t>New cases per 100,000 (Jan 18-24)</t>
-  </si>
-  <si>
-    <t>Available courses per 100,000 on Jan 24th</t>
-  </si>
-  <si>
-    <t>Population size</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Available Paxlovid</t>
-  </si>
-  <si>
-    <t>Available Molnupiravir</t>
   </si>
 </sst>
 </file>
@@ -481,12 +459,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFCCFFFF"/>
-      <color rgb="FF33CCCC"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3762,268 +3734,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0F1C6F-8999-4106-A90B-83915C46A4C3}">
-  <sheetPr>
-    <tabColor rgb="FFCCFFFF"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="3" max="3" width="32.36328125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>44564</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2.777434581424286</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1.0180469242325185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>44565</v>
-      </c>
-      <c r="B3" s="3">
-        <v>9.3024533454294112</v>
-      </c>
-      <c r="C3" s="3">
-        <v>21.170006642596007</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>44566</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5.1359963948020511</v>
-      </c>
-      <c r="C4" s="3">
-        <v>15.191383455846038</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>44568</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5.2592481051376652</v>
-      </c>
-      <c r="C5" s="3">
-        <v>19.028965793251157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>44571</v>
-      </c>
-      <c r="B6" s="3">
-        <v>6.5683399097171433</v>
-      </c>
-      <c r="C6" s="3">
-        <v>28.007425781313191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>44572</v>
-      </c>
-      <c r="B7" s="3">
-        <v>6.1750937349087183</v>
-      </c>
-      <c r="C7" s="3">
-        <v>34.888166065742375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>44573</v>
-      </c>
-      <c r="B8" s="3">
-        <v>6.4298342748350477</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44.800776393031256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>44574</v>
-      </c>
-      <c r="B9" s="3">
-        <v>7.1550058477750209</v>
-      </c>
-      <c r="C9" s="3">
-        <v>49.121908138559995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>44575</v>
-      </c>
-      <c r="B10" s="3">
-        <v>8.5382317256504319</v>
-      </c>
-      <c r="C10" s="3">
-        <v>54.481221988722602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>44580</v>
-      </c>
-      <c r="B11" s="3">
-        <v>12.846855253051041</v>
-      </c>
-      <c r="C11" s="3">
-        <v>73.25880310544764</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>44582</v>
-      </c>
-      <c r="B12" s="3">
-        <v>16.298513299430038</v>
-      </c>
-      <c r="C12" s="3">
-        <v>92.288379055680622</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>44585</v>
-      </c>
-      <c r="B13" s="3">
-        <v>17.911158202484614</v>
-      </c>
-      <c r="C13" s="3">
-        <v>103.79532957656828</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>44586</v>
-      </c>
-      <c r="B14" s="3">
-        <v>18.404775200808917</v>
-      </c>
-      <c r="C14" s="3">
-        <v>110.14096218790681</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>44587</v>
-      </c>
-      <c r="B15" s="3">
-        <v>18.124713146135424</v>
-      </c>
-      <c r="C15" s="3">
-        <v>108.94291895402561</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>44588</v>
-      </c>
-      <c r="B16" s="3">
-        <v>17.873938626591176</v>
-      </c>
-      <c r="C16" s="3">
-        <v>113.05385161930383</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>44589</v>
-      </c>
-      <c r="B17" s="3">
-        <v>18.937747324463157</v>
-      </c>
-      <c r="C17" s="3">
-        <v>116.02440088548668</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>44593</v>
-      </c>
-      <c r="B18" s="3">
-        <v>21.334138870716224</v>
-      </c>
-      <c r="C18" s="3">
-        <v>121.69336940394295</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>44596</v>
-      </c>
-      <c r="B19" s="3">
-        <v>26.941481534004687</v>
-      </c>
-      <c r="C19" s="3">
-        <v>137.53853606585142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>44599</v>
-      </c>
-      <c r="B20" s="3">
-        <v>29.592918698675007</v>
-      </c>
-      <c r="C20" s="3">
-        <v>149.14189138987282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>44601</v>
-      </c>
-      <c r="B21" s="3">
-        <v>29.976097283282755</v>
-      </c>
-      <c r="C21" s="3">
-        <v>152.09810196698203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDDF571-EC81-4645-870E-543957CFEC07}">
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4036,24 +3754,24 @@
     <col min="6" max="6" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>74</v>
+      <c r="B1" s="14">
+        <v>44602</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -4061,16 +3779,16 @@
         <v>26</v>
       </c>
       <c r="B2">
-        <v>160.00000000000003</v>
+        <v>160</v>
       </c>
       <c r="C2" s="1">
-        <v>27.475924221401002</v>
+        <v>27.475924221400998</v>
       </c>
       <c r="D2" s="1">
-        <v>1958.5182234067397</v>
+        <v>912.88758225604818</v>
       </c>
       <c r="E2" s="1">
-        <v>17.5159016911431</v>
+        <v>27.304199695017239</v>
       </c>
       <c r="F2">
         <v>582328</v>
@@ -4081,16 +3799,16 @@
         <v>27</v>
       </c>
       <c r="B3">
-        <v>479.99999999999977</v>
+        <v>480</v>
       </c>
       <c r="C3" s="1">
-        <v>26.893965498404</v>
+        <v>26.893965498404008</v>
       </c>
       <c r="D3" s="1">
-        <v>1763.6278166526315</v>
+        <v>1077.0472891162922</v>
       </c>
       <c r="E3" s="1">
-        <v>27.118081877557401</v>
+        <v>30.367769375281195</v>
       </c>
       <c r="F3">
         <v>1784787</v>
@@ -4101,16 +3819,16 @@
         <v>48</v>
       </c>
       <c r="B4">
-        <v>200.00000000000028</v>
+        <v>200</v>
       </c>
       <c r="C4" s="1">
-        <v>26.133235072369501</v>
+        <v>26.133235072369462</v>
       </c>
       <c r="D4" s="1">
-        <v>2053.5496119867921</v>
+        <v>1077.4732820337929</v>
       </c>
       <c r="E4" s="1">
-        <v>1.3066617536184699</v>
+        <v>4.3119837869409618</v>
       </c>
       <c r="F4">
         <v>765309</v>
@@ -4121,16 +3839,16 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>180.00000000000014</v>
+        <v>160</v>
       </c>
       <c r="C5" s="1">
-        <v>28.876372229272</v>
+        <v>25.667886426019535</v>
       </c>
       <c r="D5" s="1">
-        <v>2369.9480385724164</v>
+        <v>598.70345088690567</v>
       </c>
       <c r="E5" s="1">
-        <v>22.7802492030923</v>
+        <v>26.63043216699527</v>
       </c>
       <c r="F5">
         <v>623347</v>
@@ -4141,16 +3859,16 @@
         <v>45</v>
       </c>
       <c r="B6">
-        <v>359.9999999999996</v>
+        <v>360</v>
       </c>
       <c r="C6" s="1">
-        <v>25.586244834776799</v>
+        <v>25.586244834776824</v>
       </c>
       <c r="D6" s="1">
-        <v>2128.6334244487939</v>
+        <v>768.01378245721764</v>
       </c>
       <c r="E6" s="1">
-        <v>20.468995867821501</v>
+        <v>23.098693253617967</v>
       </c>
       <c r="F6">
         <v>1407006</v>
@@ -4161,16 +3879,16 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>4940.0000000000091</v>
+        <v>4920</v>
       </c>
       <c r="C7" s="1">
-        <v>25.5471749789107</v>
+        <v>25.443745120696441</v>
       </c>
       <c r="D7" s="1">
-        <v>458.96482433266021</v>
+        <v>203.56030395139294</v>
       </c>
       <c r="E7" s="1">
-        <v>22.185704586948699</v>
+        <v>37.99495841499121</v>
       </c>
       <c r="F7">
         <v>19336776</v>
@@ -4181,16 +3899,16 @@
         <v>36</v>
       </c>
       <c r="B8">
-        <v>919.99999999999864</v>
+        <v>900</v>
       </c>
       <c r="C8" s="1">
-        <v>25.864448921368101</v>
+        <v>25.302178292642743</v>
       </c>
       <c r="D8" s="1">
-        <v>852.26170549051653</v>
+        <v>283.10326156323606</v>
       </c>
       <c r="E8" s="1">
-        <v>13.775630403772199</v>
+        <v>26.061243641422028</v>
       </c>
       <c r="F8">
         <v>3557006</v>
@@ -4201,16 +3919,16 @@
         <v>40</v>
       </c>
       <c r="B9">
-        <v>1740.0000000000027</v>
+        <v>1740</v>
       </c>
       <c r="C9" s="1">
-        <v>25.240898262642901</v>
+        <v>25.240898262642862</v>
       </c>
       <c r="D9" s="1">
-        <v>1983.5284280693877</v>
+        <v>464.35999671578202</v>
       </c>
       <c r="E9" s="1">
-        <v>26.140286591541599</v>
+        <v>28.171163463248526</v>
       </c>
       <c r="F9">
         <v>6893574</v>
@@ -4221,16 +3939,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3240.0000000000041</v>
+        <v>3220</v>
       </c>
       <c r="C10" s="1">
-        <v>25.345659250766701</v>
+        <v>25.189204564033542</v>
       </c>
       <c r="D10" s="1">
-        <v>839.8878720551121</v>
+        <v>399.67131999411106</v>
       </c>
       <c r="E10" s="1">
-        <v>29.264849153431499</v>
+        <v>38.86334418450889</v>
       </c>
       <c r="F10">
         <v>12783254</v>
@@ -4241,16 +3959,16 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>359.99999999999972</v>
+        <v>340</v>
       </c>
       <c r="C11" s="1">
-        <v>26.663881772348201</v>
+        <v>25.182555007217765</v>
       </c>
       <c r="D11" s="1">
-        <v>524.38967485618173</v>
+        <v>501.28097732014658</v>
       </c>
       <c r="E11" s="1">
-        <v>25.775085713269899</v>
+        <v>14.294803283508909</v>
       </c>
       <c r="F11">
         <v>1350141</v>
@@ -4261,16 +3979,16 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>3160.0000000000018</v>
+        <v>3140</v>
       </c>
       <c r="C12" s="1">
-        <v>25.104210277949701</v>
+        <v>24.945322871127221</v>
       </c>
       <c r="D12" s="1">
-        <v>1393.1327273897261</v>
+        <v>479.75258053009611</v>
       </c>
       <c r="E12" s="1">
-        <v>19.956258296901801</v>
+        <v>33.390188543741303</v>
       </c>
       <c r="F12">
         <v>12587530</v>
@@ -4281,16 +3999,16 @@
         <v>41</v>
       </c>
       <c r="B13">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="C13" s="1">
-        <v>26.349014656639401</v>
+        <v>24.885180509048322</v>
       </c>
       <c r="D13" s="1">
-        <v>2140.271907192915</v>
+        <v>644.67255859911074</v>
       </c>
       <c r="E13" s="1">
-        <v>28.837532707544199</v>
+        <v>37.913304422608917</v>
       </c>
       <c r="F13">
         <v>1366275</v>
@@ -4301,16 +4019,16 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>2220.0000000000027</v>
+        <v>2200</v>
       </c>
       <c r="C14" s="1">
-        <v>24.993326669196801</v>
+        <v>24.768161564068873</v>
       </c>
       <c r="D14" s="1">
-        <v>776.32424945996968</v>
+        <v>270.23190091924778</v>
       </c>
       <c r="E14" s="1">
-        <v>9.9973306676787104</v>
+        <v>46.552885485193087</v>
       </c>
       <c r="F14">
         <v>8882371</v>
@@ -4321,16 +4039,16 @@
         <v>30</v>
       </c>
       <c r="B15">
-        <v>520.0000000000008</v>
+        <v>520</v>
       </c>
       <c r="C15" s="1">
-        <v>24.687618542110702</v>
+        <v>24.687618542110666</v>
       </c>
       <c r="D15" s="1">
-        <v>2548.3794240093739</v>
+        <v>910.97312420388357</v>
       </c>
       <c r="E15" s="1">
-        <v>29.055427976484101</v>
+        <v>21.744094792859013</v>
       </c>
       <c r="F15">
         <v>2106319</v>
@@ -4341,16 +4059,16 @@
         <v>42</v>
       </c>
       <c r="B16">
-        <v>2480.0000000000041</v>
+        <v>2460</v>
       </c>
       <c r="C16" s="1">
-        <v>24.883221935764201</v>
+        <v>24.682550791120903</v>
       </c>
       <c r="D16" s="1">
-        <v>1849.2949670171888</v>
+        <v>600.70907148959691</v>
       </c>
       <c r="E16" s="1">
-        <v>24.873188378531999</v>
+        <v>28.425067638717689</v>
       </c>
       <c r="F16">
         <v>9966555</v>
@@ -4361,16 +4079,16 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>179.99999999999966</v>
+        <v>180</v>
       </c>
       <c r="C17" s="1">
-        <v>24.618481914989601</v>
+        <v>24.618481914989644</v>
       </c>
       <c r="D17" s="1">
-        <v>2987.9998577598826</v>
+        <v>1658.3282956624971</v>
       </c>
       <c r="E17" s="1">
-        <v>28.3112542022381</v>
+        <v>38.705724344122608</v>
       </c>
       <c r="F17">
         <v>731158</v>
@@ -4381,16 +4099,16 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>280.00000000000011</v>
+        <v>260</v>
       </c>
       <c r="C18" s="1">
-        <v>26.4869339009105</v>
+        <v>24.595010050845453</v>
       </c>
       <c r="D18" s="1">
-        <v>1719.3803949391038</v>
+        <v>614.3076741161168</v>
       </c>
       <c r="E18" s="1">
-        <v>15.040794608017</v>
+        <v>22.135509045760909</v>
       </c>
       <c r="F18">
         <v>1057125</v>
@@ -4401,16 +4119,16 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>1100.0000000000023</v>
+        <v>1100</v>
       </c>
       <c r="C19" s="1">
-        <v>24.568647145313101</v>
+        <v>24.568647145313051</v>
       </c>
       <c r="D19" s="1">
-        <v>1751.1191577153036</v>
+        <v>1042.7827253821597</v>
       </c>
       <c r="E19" s="1">
-        <v>17.041707065339899</v>
+        <v>31.269187275852975</v>
       </c>
       <c r="F19">
         <v>4477251</v>
@@ -4421,16 +4139,16 @@
         <v>37</v>
       </c>
       <c r="B20">
-        <v>2879.9999999999964</v>
+        <v>2860</v>
       </c>
       <c r="C20" s="1">
-        <v>24.629663504919101</v>
+        <v>24.458624175023861</v>
       </c>
       <c r="D20" s="1">
-        <v>960.4200452279299</v>
+        <v>366.30638087020878</v>
       </c>
       <c r="E20" s="1">
-        <v>19.447171809092399</v>
+        <v>38.441089393962329</v>
       </c>
       <c r="F20">
         <v>11693217</v>
@@ -4441,16 +4159,16 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>1499.9999999999982</v>
+        <v>1480</v>
       </c>
       <c r="C21" s="1">
-        <v>24.769634145898401</v>
+        <v>24.439372357286452</v>
       </c>
       <c r="D21" s="1">
-        <v>530.15273616937941</v>
+        <v>196.91859145989253</v>
       </c>
       <c r="E21" s="1">
-        <v>16.744272682627301</v>
+        <v>31.044608129526033</v>
       </c>
       <c r="F21">
         <v>6055802</v>
@@ -4467,10 +4185,10 @@
         <v>24.384106244477</v>
       </c>
       <c r="D22" s="1">
-        <v>1530.2489714783985</v>
+        <v>606.61153907926916</v>
       </c>
       <c r="E22" s="1">
-        <v>24.595435165262501</v>
+        <v>34.755479433794548</v>
       </c>
       <c r="F22">
         <v>6151548</v>
@@ -4481,16 +4199,16 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>1199.9999999999993</v>
+        <v>1200</v>
       </c>
       <c r="C23" s="1">
-        <v>24.382651580849199</v>
+        <v>24.382651580849217</v>
       </c>
       <c r="D23" s="1">
-        <v>1825.6713559924024</v>
+        <v>689.58202445905056</v>
       </c>
       <c r="E23" s="1">
-        <v>18.002524417193701</v>
+        <v>22.066299680668539</v>
       </c>
       <c r="F23">
         <v>4921532</v>
@@ -4501,16 +4219,16 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>1440.0000000000016</v>
+        <v>1420</v>
       </c>
       <c r="C24" s="1">
-        <v>24.688585215480799</v>
+        <v>24.345688198599095</v>
       </c>
       <c r="D24" s="1">
-        <v>1536.4015186908878</v>
+        <v>548.36090939717849</v>
       </c>
       <c r="E24" s="1">
-        <v>23.677039015679799</v>
+        <v>41.576263296903385</v>
       </c>
       <c r="F24">
         <v>5832655</v>
@@ -4521,13 +4239,13 @@
         <v>60</v>
       </c>
       <c r="B25">
-        <v>240.00000000000034</v>
+        <v>240</v>
       </c>
       <c r="C25" s="1">
-        <v>24.320815882303499</v>
+        <v>24.320815882303467</v>
       </c>
       <c r="D25" s="1">
-        <v>1176.3167948407443</v>
+        <v>433.11319617068756</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -4541,16 +4259,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>9559.9999999999873</v>
+        <v>9560</v>
       </c>
       <c r="C26" s="1">
-        <v>24.283634065142799</v>
+        <v>24.283634065142831</v>
       </c>
       <c r="D26" s="1">
-        <v>1923.8886897145449</v>
+        <v>935.9435835297827</v>
       </c>
       <c r="E26" s="1">
-        <v>18.121280901749898</v>
+        <v>37.652333446402949</v>
       </c>
       <c r="F26">
         <v>39368078</v>
@@ -4561,16 +4279,16 @@
         <v>3</v>
       </c>
       <c r="B27">
-        <v>739.99999999999909</v>
+        <v>720</v>
       </c>
       <c r="C27" s="1">
-        <v>24.9428169069154</v>
+        <v>24.268686720242041</v>
       </c>
       <c r="D27" s="1">
-        <v>2004.3575775266568</v>
+        <v>1152.6277931741622</v>
       </c>
       <c r="E27" s="1">
-        <v>27.167446522937599</v>
+        <v>34.785117632346925</v>
       </c>
       <c r="F27">
         <v>2966786</v>
@@ -4581,16 +4299,16 @@
         <v>9</v>
       </c>
       <c r="B28">
-        <v>2099.9999999999964</v>
+        <v>2080</v>
       </c>
       <c r="C28" s="1">
-        <v>24.445429246022599</v>
+        <v>24.21261563415576</v>
       </c>
       <c r="D28" s="1">
-        <v>984.76665615513207</v>
+        <v>492.30766365370931</v>
       </c>
       <c r="E28" s="1">
-        <v>18.660010991130601</v>
+        <v>30.836162891768563</v>
       </c>
       <c r="F28">
         <v>8590563</v>
@@ -4601,16 +4319,16 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <v>1140.0000000000002</v>
+        <v>1120</v>
       </c>
       <c r="C29" s="1">
-        <v>24.540838754203701</v>
+        <v>24.110297723428193</v>
       </c>
       <c r="D29" s="1">
-        <v>1717.0406848357852</v>
+        <v>607.25659685730886</v>
       </c>
       <c r="E29" s="1">
-        <v>24.562365805742498</v>
+        <v>41.590263572913635</v>
       </c>
       <c r="F29">
         <v>4645318</v>
@@ -4621,16 +4339,16 @@
         <v>44</v>
       </c>
       <c r="B30">
-        <v>1660.0000000000023</v>
+        <v>1660</v>
       </c>
       <c r="C30" s="1">
-        <v>24.103964172796999</v>
+        <v>24.103964172796964</v>
       </c>
       <c r="D30" s="1">
-        <v>1672.6844294490038</v>
+        <v>1197.8944170862837</v>
       </c>
       <c r="E30" s="1">
-        <v>19.370294100307898</v>
+        <v>20.183439879631191</v>
       </c>
       <c r="F30">
         <v>6886834</v>
@@ -4641,16 +4359,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>259.99999999999983</v>
+        <v>260</v>
       </c>
       <c r="C31" s="1">
-        <v>24.061219144956802</v>
+        <v>24.061219144956816</v>
       </c>
       <c r="D31" s="1">
-        <v>1389.6279487718136</v>
+        <v>1039.0744944599044</v>
       </c>
       <c r="E31" s="1">
-        <v>13.788929433071401</v>
+        <v>30.354153382868596</v>
       </c>
       <c r="F31">
         <v>1080577</v>
@@ -4661,16 +4379,16 @@
         <v>46</v>
       </c>
       <c r="B32">
-        <v>1039.9999999999984</v>
+        <v>1020</v>
       </c>
       <c r="C32" s="1">
-        <v>24.519587024140201</v>
+        <v>24.048056504445235</v>
       </c>
       <c r="D32" s="1">
-        <v>1812.5397411816132</v>
+        <v>794.31673695222003</v>
       </c>
       <c r="E32" s="1">
-        <v>9.3598808159458393</v>
+        <v>20.134353190976697</v>
       </c>
       <c r="F32">
         <v>4241507</v>
@@ -4681,16 +4399,16 @@
         <v>15</v>
       </c>
       <c r="B33">
-        <v>1359.999999999998</v>
+        <v>1360</v>
       </c>
       <c r="C33" s="1">
-        <v>24.039557799404701</v>
+        <v>24.03955779940474</v>
       </c>
       <c r="D33" s="1">
-        <v>1612.029111904495</v>
+        <v>873.0778517544104</v>
       </c>
       <c r="E33" s="1">
-        <v>19.496788421134902</v>
+        <v>45.851921273276389</v>
       </c>
       <c r="F33">
         <v>5657342</v>
@@ -4701,16 +4419,16 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>700.00000000000102</v>
+        <v>700</v>
       </c>
       <c r="C34" s="1">
-        <v>24.0235705546528</v>
+        <v>24.023570554652768</v>
       </c>
       <c r="D34" s="1">
-        <v>2553.4309948675359</v>
+        <v>743.6667862125297</v>
       </c>
       <c r="E34" s="1">
-        <v>9.47215067583452</v>
+        <v>19.493411535775387</v>
       </c>
       <c r="F34">
         <v>2913805</v>
@@ -4721,16 +4439,16 @@
         <v>11</v>
       </c>
       <c r="B35">
-        <v>780.00000000000011</v>
+        <v>760</v>
       </c>
       <c r="C35" s="1">
-        <v>24.655759759334501</v>
+        <v>24.023560791146434</v>
       </c>
       <c r="D35" s="1">
-        <v>1162.2345831169368</v>
+        <v>550.3924217045286</v>
       </c>
       <c r="E35" s="1">
-        <v>27.247775528905599</v>
+        <v>39.133116130841167</v>
       </c>
       <c r="F35">
         <v>3163561</v>
@@ -4741,16 +4459,16 @@
         <v>43</v>
       </c>
       <c r="B36">
-        <v>5239.9999999999991</v>
+        <v>5220</v>
       </c>
       <c r="C36" s="1">
-        <v>24.110453114555199</v>
+        <v>24.018428484346977</v>
       </c>
       <c r="D36" s="1">
-        <v>1057.6666823722035</v>
+        <v>594.02819045711942</v>
       </c>
       <c r="E36" s="1">
-        <v>7.5552221400953501</v>
+        <v>12.133447492954595</v>
       </c>
       <c r="F36">
         <v>21733312</v>
@@ -4761,16 +4479,16 @@
         <v>22</v>
       </c>
       <c r="B37">
-        <v>2519.9999999999959</v>
+        <v>2520</v>
       </c>
       <c r="C37" s="1">
-        <v>23.771739231944501</v>
+        <v>23.771739231944537</v>
       </c>
       <c r="D37" s="1">
-        <v>1589.4803639302347</v>
+        <v>899.70373054997708</v>
       </c>
       <c r="E37" s="1">
-        <v>15.423330811202099</v>
+        <v>26.196079304408727</v>
       </c>
       <c r="F37">
         <v>10600823</v>
@@ -4781,16 +4499,16 @@
         <v>28</v>
       </c>
       <c r="B38">
-        <v>739.99999999999989</v>
+        <v>720</v>
       </c>
       <c r="C38" s="1">
-        <v>24.418235538299999</v>
+        <v>23.758283226454054</v>
       </c>
       <c r="D38" s="1">
-        <v>1884.3288383981373</v>
+        <v>781.02056345408482</v>
       </c>
       <c r="E38" s="1">
-        <v>20.887490669924201</v>
+        <v>22.537371449539059</v>
       </c>
       <c r="F38">
         <v>3030522</v>
@@ -4801,16 +4519,16 @@
         <v>33</v>
       </c>
       <c r="B39">
-        <v>460.0000000000004</v>
+        <v>460</v>
       </c>
       <c r="C39" s="1">
-        <v>23.741298298058599</v>
+        <v>23.741298298058581</v>
       </c>
       <c r="D39" s="1">
-        <v>1477.1216462835578</v>
+        <v>538.56619073965499</v>
       </c>
       <c r="E39" s="1">
-        <v>10.3739151258908</v>
+        <v>20.696218733742374</v>
       </c>
       <c r="F39">
         <v>1937552</v>
@@ -4821,16 +4539,16 @@
         <v>19</v>
       </c>
       <c r="B40">
-        <v>1619.999999999998</v>
+        <v>1600</v>
       </c>
       <c r="C40" s="1">
-        <v>23.982402246174001</v>
+        <v>23.686323206097807</v>
       </c>
       <c r="D40" s="1">
-        <v>1445.7687566441987</v>
+        <v>634.57140264336408</v>
       </c>
       <c r="E40" s="1">
-        <v>22.946125605907302</v>
+        <v>34.552423976895177</v>
       </c>
       <c r="F40">
         <v>6754953</v>
@@ -4841,16 +4559,16 @@
         <v>16</v>
       </c>
       <c r="B41">
-        <v>1819.9999999999984</v>
+        <v>1820</v>
       </c>
       <c r="C41" s="1">
-        <v>23.655988890523702</v>
+        <v>23.655988890523723</v>
       </c>
       <c r="D41" s="1">
-        <v>2103.7582867448996</v>
+        <v>952.36151758107883</v>
       </c>
       <c r="E41" s="1">
-        <v>13.582696917910599</v>
+        <v>45.570273104492401</v>
       </c>
       <c r="F41">
         <v>7693612</v>
@@ -4861,16 +4579,16 @@
         <v>23</v>
       </c>
       <c r="B42">
-        <v>960.00000000000057</v>
+        <v>940</v>
       </c>
       <c r="C42" s="1">
-        <v>24.1158586137451</v>
+        <v>23.613444892625395</v>
       </c>
       <c r="D42" s="1">
-        <v>2006.5901607799269</v>
+        <v>801.12379901140059</v>
       </c>
       <c r="E42" s="1">
-        <v>19.744859240003802</v>
+        <v>32.1795988377161</v>
       </c>
       <c r="F42">
         <v>3980783</v>
@@ -4881,16 +4599,16 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>1360.0000000000023</v>
+        <v>1360</v>
       </c>
       <c r="C43" s="1">
-        <v>23.417110917384299</v>
+        <v>23.41711091738426</v>
       </c>
       <c r="D43" s="1">
-        <v>1281.0020595004682</v>
+        <v>512.71419984334648</v>
       </c>
       <c r="E43" s="1">
-        <v>20.6449382278998</v>
+        <v>28.720397801615398</v>
       </c>
       <c r="F43">
         <v>5807719</v>
@@ -4901,16 +4619,16 @@
         <v>25</v>
       </c>
       <c r="B44">
-        <v>1239.9999999999989</v>
+        <v>1220</v>
       </c>
       <c r="C44" s="1">
-        <v>23.763712045135701</v>
+        <v>23.380426366988374</v>
       </c>
       <c r="D44" s="1">
-        <v>1995.2510904477544</v>
+        <v>864.32836850618253</v>
       </c>
       <c r="E44" s="1">
-        <v>20.889069459030601</v>
+        <v>6.5733493802270591</v>
       </c>
       <c r="F44">
         <v>5218040</v>
@@ -4921,16 +4639,16 @@
         <v>34</v>
       </c>
       <c r="B45">
-        <v>2500.0000000000041</v>
+        <v>2480</v>
       </c>
       <c r="C45" s="1">
-        <v>23.342633349694999</v>
+        <v>23.155892282897401</v>
       </c>
       <c r="D45" s="1">
-        <v>1157.729254771491</v>
+        <v>528.5425784104732</v>
       </c>
       <c r="E45" s="1">
-        <v>15.406138010798699</v>
+        <v>11.512586768069555</v>
       </c>
       <c r="F45">
         <v>10710017</v>
@@ -4941,16 +4659,16 @@
         <v>7</v>
       </c>
       <c r="B46">
-        <v>720.00000000000034</v>
+        <v>720</v>
       </c>
       <c r="C46" s="1">
-        <v>22.9426570592166</v>
+        <v>22.942657059216589</v>
       </c>
       <c r="D46" s="1">
-        <v>1834.5840798990778</v>
+        <v>545.62099559023011</v>
       </c>
       <c r="E46" s="1">
-        <v>12.650326184040299</v>
+        <v>38.428950574187787</v>
       </c>
       <c r="F46">
         <v>3138259</v>
@@ -4961,16 +4679,16 @@
         <v>35</v>
       </c>
       <c r="B47">
-        <v>1699.999999999998</v>
+        <v>1700</v>
       </c>
       <c r="C47" s="1">
-        <v>22.906726101985299</v>
+        <v>22.906726101985324</v>
       </c>
       <c r="D47" s="1">
-        <v>1959.7916889277374</v>
+        <v>997.19715994325065</v>
       </c>
       <c r="E47" s="1">
-        <v>20.589104402255</v>
+        <v>27.757562217699867</v>
       </c>
       <c r="F47">
         <v>7421401</v>
@@ -4981,16 +4699,16 @@
         <v>39</v>
       </c>
       <c r="B48">
-        <v>219.99999999999986</v>
+        <v>200</v>
       </c>
       <c r="C48" s="1">
-        <v>24.643868101537201</v>
+        <v>22.403516455942924</v>
       </c>
       <c r="D48" s="1">
-        <v>1725.7428726012836</v>
+        <v>544.06939713257395</v>
       </c>
       <c r="E48" s="1">
-        <v>13.106057126726601</v>
+        <v>16.354567012838338</v>
       </c>
       <c r="F48">
         <v>892717</v>
@@ -5001,16 +4719,16 @@
         <v>13</v>
       </c>
       <c r="B49">
-        <v>6559.9999999999918</v>
+        <v>6540</v>
       </c>
       <c r="C49" s="1">
-        <v>22.3427466571964</v>
+        <v>22.274628527144003</v>
       </c>
       <c r="D49" s="1">
-        <v>1303.508536683265</v>
+        <v>708.64993646792311</v>
       </c>
       <c r="E49" s="1">
-        <v>11.147531983079899</v>
+        <v>19.835999471267073</v>
       </c>
       <c r="F49">
         <v>29360759</v>
@@ -5021,16 +4739,16 @@
         <v>18</v>
       </c>
       <c r="B50">
-        <v>400.00000000000017</v>
+        <v>400</v>
       </c>
       <c r="C50" s="1">
-        <v>21.894857609530401</v>
+        <v>21.894857609530394</v>
       </c>
       <c r="D50" s="1">
-        <v>1105.7997835693325</v>
+        <v>745.51990160450998</v>
       </c>
       <c r="E50" s="1">
-        <v>9.7432116362410195</v>
+        <v>23.318023354149869</v>
       </c>
       <c r="F50">
         <v>1826913</v>
@@ -5041,16 +4759,16 @@
         <v>14</v>
       </c>
       <c r="B51">
-        <v>679.99999999999898</v>
+        <v>680</v>
       </c>
       <c r="C51" s="1">
-        <v>20.9238559343286</v>
+        <v>20.923855934328632</v>
       </c>
       <c r="D51" s="1">
-        <v>3003.9579935129896</v>
+        <v>708.21098262427608</v>
       </c>
       <c r="E51" s="1">
-        <v>6.2156160275505599</v>
+        <v>11.631202269376798</v>
       </c>
       <c r="F51">
         <v>3249879</v>
@@ -5061,12 +4779,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE68B34-216F-45D0-AB9C-A3900E967393}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5083,43 +4801,43 @@
         <v>68</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" s="10">
-        <f>CORREL(CorrelationData!$B$2:$B$51,CorrelationData!$F$2:$F$51)</f>
-        <v>0.99853900841111332</v>
+        <f>CORREL(CorrelationData!$B$2:$B$51,CorrelationData!$F$2:$F$51)^2</f>
+        <v>0.99713386703576223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="10">
-        <f>CORREL(CorrelationData!$C$2:$C$51,CorrelationData!$D$2:$D$51)</f>
-        <v>-5.3457852500284564E-2</v>
+        <f>CORREL(CorrelationData!$C$2:$C$51,CorrelationData!$D$2:$D$51)^2</f>
+        <v>2.9302971990234085E-4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>69</v>
       </c>
       <c r="C4" s="11">
-        <f>CORREL(CorrelationData!$C$2:$C$51,CorrelationData!$E$2:$E$51)</f>
-        <v>0.35728886057403908</v>
+        <f>CORREL(CorrelationData!$C$2:$C$51,CorrelationData!$E$2:$E$51)^2</f>
+        <v>2.5138247849899351E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>